<commit_message>
Refactor : ItemSO, WeaponData 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BF2776-501A-49A0-97B2-F6A7A5F01C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D376C02-9D1C-46A1-9F86-F2D34A0BC3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -51,63 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>itemName</t>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>iconWidth</t>
-  </si>
-  <si>
-    <t>iconHeight</t>
-  </si>
-  <si>
-    <t>itemPrefab</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>atk</t>
-  </si>
-  <si>
-    <t>atkRate</t>
-  </si>
-  <si>
-    <t>critRate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>critDamage</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>lifeSteal</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>weaponTier</t>
-  </si>
-  <si>
-    <t>projectile</t>
-  </si>
-  <si>
-    <t>numberOfProjectile</t>
-  </si>
-  <si>
     <t>Axe</t>
   </si>
   <si>
@@ -131,6 +74,61 @@
   <si>
     <t>None</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_name</t>
+  </si>
+  <si>
+    <t>_description</t>
+  </si>
+  <si>
+    <t>_spritePath</t>
+  </si>
+  <si>
+    <t>_iconWidth</t>
+  </si>
+  <si>
+    <t>_iconHeight</t>
+  </si>
+  <si>
+    <t>_prefabPath</t>
+  </si>
+  <si>
+    <t>_price</t>
+  </si>
+  <si>
+    <t>_atk</t>
+  </si>
+  <si>
+    <t>_atkRate</t>
+  </si>
+  <si>
+    <t>_critRate</t>
+  </si>
+  <si>
+    <t>_critDamage</t>
+  </si>
+  <si>
+    <t>_range</t>
+  </si>
+  <si>
+    <t>_lifeSteal</t>
+  </si>
+  <si>
+    <t>_type</t>
+  </si>
+  <si>
+    <t>_weaponTier</t>
+  </si>
+  <si>
+    <t>_projectilePath</t>
+  </si>
+  <si>
+    <t>_numberOfProjectile</t>
   </si>
 </sst>
 </file>
@@ -496,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -515,58 +513,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="Q1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="R1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -574,13 +572,13 @@
         <v>110001</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -589,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>24</v>
@@ -613,13 +611,13 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -630,13 +628,13 @@
         <v>110011</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -645,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>30</v>
@@ -669,13 +667,13 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="R3">
         <v>0</v>

</xml_diff>

<commit_message>
Docs : ItemSO, WeaponDB 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D376C02-9D1C-46A1-9F86-F2D34A0BC3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E540549-9C84-41BD-A0C5-974A43485864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,13 +122,26 @@
     <t>_type</t>
   </si>
   <si>
-    <t>_weaponTier</t>
-  </si>
-  <si>
     <t>_projectilePath</t>
   </si>
   <si>
     <t>_numberOfProjectile</t>
+  </si>
+  <si>
+    <t>_grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -492,21 +505,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
     <col min="4" max="4" width="21.625" customWidth="1"/>
     <col min="5" max="5" width="11.75" customWidth="1"/>
     <col min="6" max="6" width="12.125" customWidth="1"/>
     <col min="7" max="7" width="33.5" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="16" max="16" width="12.875" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
     <col min="17" max="17" width="21.5" customWidth="1"/>
     <col min="18" max="18" width="18.5" customWidth="1"/>
   </cols>
@@ -537,39 +550,39 @@
         <v>21</v>
       </c>
       <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>110001</v>
+        <v>10001011</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -592,12 +605,12 @@
       <c r="H2">
         <v>24</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
         <v>1</v>
       </c>
@@ -605,16 +618,16 @@
         <v>1</v>
       </c>
       <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>3</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>10</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
       </c>
       <c r="Q2" t="s">
         <v>13</v>
@@ -625,13 +638,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>110011</v>
+        <v>10001012</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -640,20 +653,20 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
       <c r="H3">
-        <v>30</v>
-      </c>
-      <c r="I3">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>0.7</v>
-      </c>
       <c r="K3">
         <v>1</v>
       </c>
@@ -661,16 +674,16 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>10</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
       </c>
       <c r="Q3" t="s">
         <v>13</v>
@@ -681,57 +694,169 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>120001</v>
+        <v>10001013</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10002011</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0.7</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20001011</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="H6">
         <v>35</v>
       </c>
-      <c r="I4">
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="K6">
         <v>0.7</v>
       </c>
-      <c r="K4">
+      <c r="L6">
         <v>5</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>10</v>
       </c>
-      <c r="N4">
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P6" t="s">
         <v>0</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="Q6" t="s">
         <v>5</v>
       </c>
-      <c r="R4">
+      <c r="R6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor : 임시 무기 Asset 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E540549-9C84-41BD-A0C5-974A43485864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50159B19-CCD5-460B-91CC-098ADFAFE112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,12 +57,6 @@
     <t>발등 조심하세요.</t>
   </si>
   <si>
-    <t>Resources/Icons/Weapons</t>
-  </si>
-  <si>
-    <t>Resources/Prefabs/Weapons</t>
-  </si>
-  <si>
     <t>Melee</t>
   </si>
   <si>
@@ -141,6 +135,18 @@
   </si>
   <si>
     <t>Unique</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Icons/Weapons/Axe_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Icons/Weapons/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Prefabs/Weapons/Axe_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -508,14 +514,14 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="4" max="4" width="30.75" customWidth="1"/>
     <col min="5" max="5" width="11.75" customWidth="1"/>
     <col min="6" max="6" width="12.125" customWidth="1"/>
     <col min="7" max="7" width="33.5" customWidth="1"/>
@@ -526,58 +532,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -591,7 +597,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -600,13 +606,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="H2">
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -627,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -647,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -656,13 +662,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="H3">
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -683,10 +689,10 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -703,7 +709,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -712,13 +718,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="H4">
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -739,10 +745,10 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -753,13 +759,13 @@
         <v>10002011</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -768,13 +774,13 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -795,10 +801,10 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -830,7 +836,7 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J6">
         <v>3</v>

</xml_diff>

<commit_message>
Feature : Weapon Sprite, Prefab 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50159B19-CCD5-460B-91CC-098ADFAFE112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C17146-2441-4AFC-A41C-C40A2CF841AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -25,20 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Resources/Items/Icons/Weapon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resources/Items/Prefabs/Weapons/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Bow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,15 +130,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Resources/Items/Icons/Weapons/Axe_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resources/Items/Icons/Weapons/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resources/Items/Prefabs/Weapons/Axe_1</t>
+    <t>Resources/Items/Icons/Weapons/Melee/Axe_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Icons/Weapons/Melee/Spear1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Icons/Weapon/Range/Bow_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Prefabs/Weapons/Melee/Axe_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Prefabs/Weapons/Melee/Spear_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Items/Prefabs/Weapons/Range/Bow_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -514,76 +518,76 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="30.75" customWidth="1"/>
+    <col min="4" max="4" width="39.625" customWidth="1"/>
     <col min="5" max="5" width="11.75" customWidth="1"/>
     <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="7" width="33.5" customWidth="1"/>
+    <col min="7" max="7" width="42.75" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="17" max="17" width="21.5" customWidth="1"/>
+    <col min="17" max="17" width="31.5" customWidth="1"/>
     <col min="18" max="18" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -591,13 +595,13 @@
         <v>10001011</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -606,13 +610,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2">
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -633,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -647,13 +651,13 @@
         <v>10001012</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -662,13 +666,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3">
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -689,10 +693,10 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -703,13 +707,13 @@
         <v>10001013</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -718,13 +722,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -745,10 +749,10 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -759,13 +763,13 @@
         <v>10002011</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -774,13 +778,13 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="H5">
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -801,10 +805,10 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -815,13 +819,13 @@
         <v>20001011</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -830,13 +834,13 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -860,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R6">
         <v>1</v>

</xml_diff>

<commit_message>
Feature : 화살 ObjectPooling 구현
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C17146-2441-4AFC-A41C-C40A2CF841AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5507EE03-4159-454E-A68B-CBA8BF9B8734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="38400" yWindow="2445" windowWidth="28800" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Resources/Items/Prefabs/Projectiles/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Axe</t>
   </si>
   <si>
@@ -108,9 +104,6 @@
     <t>_type</t>
   </si>
   <si>
-    <t>_projectilePath</t>
-  </si>
-  <si>
     <t>_numberOfProjectile</t>
   </si>
   <si>
@@ -151,6 +144,14 @@
   </si>
   <si>
     <t>Resources/Items/Prefabs/Weapons/Range/Bow_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_projectileTag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arrow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,7 +519,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -536,58 +537,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
         <v>24</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -595,13 +596,13 @@
         <v>10001011</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -610,13 +611,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2">
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -637,10 +638,10 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -651,13 +652,13 @@
         <v>10001012</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -666,13 +667,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3">
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -693,10 +694,10 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -707,13 +708,13 @@
         <v>10001013</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -722,13 +723,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -749,10 +750,10 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -763,13 +764,13 @@
         <v>10002011</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -778,13 +779,13 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5">
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -805,10 +806,10 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -825,7 +826,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -834,13 +835,13 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6">
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -864,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="R6">
         <v>1</v>

</xml_diff>

<commit_message>
Featrue : Bow_1 구현
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5507EE03-4159-454E-A68B-CBA8BF9B8734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AE5A08-D591-4E0E-9EA9-C13701541D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="2445" windowWidth="28800" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -868,7 +868,7 @@
         <v>36</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove : 필요 없는 아이템 ScriptableObject 삭제
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SpartaCoding\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCE8612-11A6-44C0-88AB-8C1798F434E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09914BD2-6612-45E2-A743-7F2D5EB3A451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="780" windowWidth="26490" windowHeight="14025" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="1095" yWindow="7125" windowWidth="26490" windowHeight="8070" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -153,10 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Items/Icons/Weapons/Melee/Spear1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Items/Prefabs/Weapons/Melee/Axe_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -178,6 +174,10 @@
   </si>
   <si>
     <t>Items/Icons/Weapons/Range/Wand_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Melee/Spear_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,7 +545,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -641,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2">
         <v>24</v>
@@ -700,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3">
         <v>24</v>
@@ -759,7 +759,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4">
         <v>24</v>
@@ -809,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -818,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5">
         <v>30</v>
@@ -868,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6">
         <v>35</v>
@@ -927,7 +927,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -936,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7">
         <v>35</v>

</xml_diff>

<commit_message>
Feat : ItemData에 id 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SpartaCoding\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09914BD2-6612-45E2-A743-7F2D5EB3A451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C7850E-F41C-4359-8102-44CBD93D38A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="7125" windowWidth="26490" windowHeight="8070" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="1935" yWindow="5160" windowWidth="26640" windowHeight="8550" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix : spear 오탈 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SpartaCoding\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA89B0A9-C0AC-487B-B54A-04B94EDEA411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C60B85-1BD4-495C-9025-152CBFC5AF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="645" yWindow="5385" windowWidth="26640" windowHeight="8550" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -153,10 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Items/Icons/Weapons/Melee/Spear1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Items/Prefabs/Weapons/Melee/Axe_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -186,6 +182,10 @@
   </si>
   <si>
     <t>Weapon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Melee/Spear_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -254,9 +254,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +294,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -400,7 +400,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,7 +553,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -576,7 +576,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -638,7 +638,7 @@
         <v>10111011</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -656,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <v>24</v>
@@ -700,7 +700,7 @@
         <v>10111012</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3">
         <v>24</v>
@@ -762,7 +762,7 @@
         <v>10111013</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -780,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4">
         <v>24</v>
@@ -824,7 +824,7 @@
         <v>10112013</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -833,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -842,7 +842,7 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5">
         <v>30</v>
@@ -886,7 +886,7 @@
         <v>10121011</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -895,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -904,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6">
         <v>35</v>
@@ -948,7 +948,7 @@
         <v>10122011</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
@@ -957,7 +957,7 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -966,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7">
         <v>35</v>

</xml_diff>

<commit_message>
Feature : 근접 무기 Sword 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SpartaCoding\Sisyphus\Assets\Excel\Items\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C60B85-1BD4-495C-9025-152CBFC5AF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19B6BBD-18C6-4D38-9185-D126605F4601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="5385" windowWidth="26640" windowHeight="8550" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,6 +186,22 @@
   </si>
   <si>
     <t>Items/Icons/Weapons/Melee/Spear_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Melee/Sword_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Prefabs/Weapons/Melee/Sword_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -254,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -400,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,17 +566,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="20.25" customWidth="1"/>
     <col min="5" max="5" width="39.625" customWidth="1"/>
     <col min="6" max="6" width="11.75" customWidth="1"/>
     <col min="7" max="7" width="12.125" customWidth="1"/>
@@ -821,19 +837,19 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>10112013</v>
+        <v>10112011</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -842,22 +858,22 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -883,37 +899,37 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>10121011</v>
+        <v>10113011</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
         <v>24</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -922,51 +938,51 @@
         <v>0.7</v>
       </c>
       <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
         <v>5</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6" t="s">
-        <v>0</v>
-      </c>
       <c r="S6" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>10122011</v>
+        <v>10121011</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7">
         <v>35</v>
@@ -975,13 +991,13 @@
         <v>24</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N7">
         <v>5</v>
@@ -999,9 +1015,71 @@
         <v>0</v>
       </c>
       <c r="S7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10122011</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8">
+        <v>35</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
         <v>34</v>
       </c>
-      <c r="T7">
+      <c r="T8">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature : Tutorial 프리팹 생성
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E76755F-3822-49F0-8462-D1293E7E4BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E7E8EB-724D-4D2F-B6CC-E42570E99540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Docs : WeaponDB_Sheet에 Particle 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Items\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8675DDA-34A4-4C20-A3B1-E262AF86D93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1446A1DB-A439-443A-82AF-F6E8C30F142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="30" yWindow="315" windowWidth="37440" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,6 +220,10 @@
   </si>
   <si>
     <t>Arrow_Ricochet</t>
+  </si>
+  <si>
+    <t>_particleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -287,9 +291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,7 +331,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -433,7 +437,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -575,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -583,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -603,9 +607,10 @@
     <col min="20" max="20" width="31.5" customWidth="1"/>
     <col min="21" max="21" width="18.5" customWidth="1"/>
     <col min="22" max="22" width="15.125" customWidth="1"/>
+    <col min="23" max="23" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -672,8 +677,11 @@
       <c r="V1" t="s">
         <v>45</v>
       </c>
+      <c r="W1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10111011</v>
       </c>
@@ -740,8 +748,11 @@
       <c r="V2" t="s">
         <v>46</v>
       </c>
+      <c r="W2">
+        <v>71000002</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10111012</v>
       </c>
@@ -808,8 +819,11 @@
       <c r="V3" t="s">
         <v>46</v>
       </c>
+      <c r="W3">
+        <v>71000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10111013</v>
       </c>
@@ -876,8 +890,11 @@
       <c r="V4" t="s">
         <v>46</v>
       </c>
+      <c r="W4">
+        <v>71000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10112011</v>
       </c>
@@ -944,8 +961,11 @@
       <c r="V5" t="s">
         <v>47</v>
       </c>
+      <c r="W5">
+        <v>71000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10112012</v>
       </c>
@@ -1012,8 +1032,11 @@
       <c r="V6" t="s">
         <v>47</v>
       </c>
+      <c r="W6">
+        <v>71000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10112013</v>
       </c>
@@ -1080,8 +1103,11 @@
       <c r="V7" t="s">
         <v>47</v>
       </c>
+      <c r="W7">
+        <v>71000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10121011</v>
       </c>
@@ -1149,7 +1175,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10121012</v>
       </c>
@@ -1217,7 +1243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10121013</v>
       </c>
@@ -1285,7 +1311,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10122011</v>
       </c>
@@ -1353,7 +1379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10122012</v>
       </c>
@@ -1421,7 +1447,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10122013</v>
       </c>

</xml_diff>

<commit_message>
Feature : Epic 등급 무기 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1446A1DB-A439-443A-82AF-F6E8C30F142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080CE8C7-57E4-4BEA-A579-17E4B94662E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="315" windowWidth="37440" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -25,26 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="80">
   <si>
     <t>Range</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Bow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>활.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Axe</t>
-  </si>
-  <si>
-    <t>발등 조심하세요.</t>
-  </si>
-  <si>
     <t>Melee</t>
   </si>
   <si>
@@ -111,14 +97,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Wand</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>완드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>_magicAtk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,14 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>칼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Items/Icons/Weapons/Melee/Sword_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -213,9 +183,6 @@
   </si>
   <si>
     <t>Items/Prefabs/Weapons/Melee/Sword_1</t>
-  </si>
-  <si>
-    <t>Items/Prefabs/Weapons/Melee/Sword_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -223,6 +190,142 @@
   </si>
   <si>
     <t>_particleID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>믿는 도끼에 발 등 찍힌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>믿지 않으면 발 등에 안 찍히나?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무꾼은 테스트 해보기 위해 도끼를 던졌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맙소사! 도끼는 날아가 산신령을 찍었다!
+- 라는 전설이 내려오는 전설의 도끼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무꾼의 도끼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동 추적 도끼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평범한 칼이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강타의 거인</t>
+  </si>
+  <si>
+    <t>쌍검의 분노</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평범한 칼이다. 어느 왕국의 왕이 사용하던 검의 레플리카이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평범한 칼이다. 어라? 여기 버튼이 있는데?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검을 쪼개버린 이상 우물까지 간다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강타의 거인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>섬광 스트라이커</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chat GPT야, 활에 대한 이름을 지어줘.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어때요, 마음에 드시나요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아직 AI는 갈 길이 먼 것 같네.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 거는 없어?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위더스트링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에테리얼 스태프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>룬웨이버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신비로우면서도 고귀하고 우아한 느낌의 스태프.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원소의 힘으로 큐브를 생성해 공격한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주인이 성장함에 따라 스태프 또한 성장하는 듯 하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법에 통달한 자만이 사용할 수 있다는 전설의 스태프. 아니, 완드인가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Melee/Sword_1_Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Range/Bow_1_Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Range/Wand_1_Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Weapons/Melee/Axe_1_Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Prefabs/Weapons/Melee/Sword_1_Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Prefabs/Weapons/Melee/Sword_1_Unique</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Prefabs/Weapons/Melee/Axe_1_Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Prefabs/Weapons/Melee/Axe_1_Unique</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -269,9 +372,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,17 +693,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.625" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="30.875" customWidth="1"/>
+    <col min="4" max="4" width="63.25" customWidth="1"/>
     <col min="5" max="5" width="39.625" customWidth="1"/>
     <col min="6" max="6" width="11.75" customWidth="1"/>
     <col min="7" max="7" width="12.125" customWidth="1"/>
@@ -612,73 +719,73 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
       <c r="V1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" t="s">
         <v>45</v>
-      </c>
-      <c r="W1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -686,16 +793,16 @@
         <v>10111011</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -704,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I2">
         <v>24</v>
@@ -713,7 +820,7 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L2">
         <v>30</v>
@@ -734,19 +841,19 @@
         <v>5</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="W2">
         <v>71000002</v>
@@ -757,16 +864,16 @@
         <v>10111012</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -775,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="I3">
         <v>48</v>
@@ -784,10 +891,10 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -796,28 +903,28 @@
         <v>1</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q3">
         <v>5</v>
       </c>
       <c r="R3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="W3">
         <v>71000002</v>
@@ -828,16 +935,16 @@
         <v>10111013</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -846,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="I4">
         <v>96</v>
@@ -855,10 +962,10 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L4">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -867,69 +974,69 @@
         <v>1</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q4">
         <v>5</v>
       </c>
       <c r="R4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="W4">
         <v>71000002</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="33" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>10112011</v>
+        <v>10111014</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="I5">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="L5">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -938,69 +1045,69 @@
         <v>1</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q5">
         <v>5</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="W5">
-        <v>71000001</v>
+        <v>71000002</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>10112012</v>
+        <v>10112011</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
         <v>43</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
       <c r="I6">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="J6">
         <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L6">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1009,28 +1116,28 @@
         <v>1</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <v>5</v>
       </c>
       <c r="R6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="W6">
         <v>71000001</v>
@@ -1038,19 +1145,19 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>10112013</v>
+        <v>10112012</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1059,19 +1166,19 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="I7">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="J7">
         <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L7">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1080,28 +1187,28 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q7">
         <v>5</v>
       </c>
       <c r="R7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U7">
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="W7">
         <v>71000001</v>
@@ -1109,155 +1216,161 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>10121011</v>
+        <v>10112013</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8">
+        <v>112</v>
+      </c>
+      <c r="J8">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8">
-        <v>35</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <v>0.7</v>
-      </c>
-      <c r="O8">
-        <v>5</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>10</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>53</v>
-      </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="W8">
+        <v>71000001</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>10121012</v>
+        <v>10112014</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9">
-        <v>70</v>
-      </c>
-      <c r="J9">
-        <v>10</v>
-      </c>
-      <c r="K9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>25</v>
-      </c>
-      <c r="N9">
-        <v>0.6</v>
-      </c>
-      <c r="O9">
-        <v>5</v>
-      </c>
-      <c r="P9">
-        <v>2</v>
-      </c>
-      <c r="Q9">
-        <v>10</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9" t="s">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>31</v>
-      </c>
       <c r="U9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="W9">
+        <v>71000001</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>10121013</v>
+        <v>10121011</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1266,31 +1379,31 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10">
         <v>35</v>
-      </c>
-      <c r="I10">
-        <v>140</v>
       </c>
       <c r="J10">
         <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="N10">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="O10">
         <v>5</v>
       </c>
       <c r="P10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <v>10</v>
@@ -1302,63 +1415,63 @@
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="U10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10122011</v>
+        <v>10121012</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11">
+        <v>70</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11">
-        <v>35</v>
-      </c>
-      <c r="J11">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>20</v>
-      </c>
       <c r="N11">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="O11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q11">
         <v>10</v>
@@ -1370,63 +1483,63 @@
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="U11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10122012</v>
+        <v>10121013</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I12">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="J12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q12">
         <v>10</v>
@@ -1438,63 +1551,63 @@
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="U12">
         <v>3</v>
       </c>
       <c r="V12" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>10122013</v>
+        <v>10121014</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="I13">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>60</v>
+      </c>
+      <c r="N13">
+        <v>0.5</v>
+      </c>
+      <c r="O13">
         <v>15</v>
       </c>
-      <c r="K13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>50</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>5</v>
-      </c>
       <c r="P13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q13">
         <v>10</v>
@@ -1506,13 +1619,285 @@
         <v>0</v>
       </c>
       <c r="T13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10122011</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="U13">
-        <v>3</v>
-      </c>
-      <c r="V13" t="s">
-        <v>48</v>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>35</v>
+      </c>
+      <c r="J14">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>10122012</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <v>70</v>
+      </c>
+      <c r="J15">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>45</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>26</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10122013</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16">
+        <v>90</v>
+      </c>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>60</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16">
+        <v>3</v>
+      </c>
+      <c r="V16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10122013</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>90</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>10</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>26</v>
+      </c>
+      <c r="U17">
+        <v>3</v>
+      </c>
+      <c r="V17" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature : Sword의 무기 스킬 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE825EF2-3D38-400E-8833-F9CF96CE6D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFCC14A-24C9-48C7-9E5C-09173BDA3663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="375" yWindow="660" windowWidth="37440" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -724,7 +724,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="Q2" sqref="Q2:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>3</v>
       </c>
       <c r="Q3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -1008,7 +1008,7 @@
         <v>5</v>
       </c>
       <c r="Q4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -1079,7 +1079,7 @@
         <v>5</v>
       </c>
       <c r="Q5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R5">
         <v>5</v>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R6">
         <v>1</v>
@@ -1221,7 +1221,7 @@
         <v>3</v>
       </c>
       <c r="Q7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R7">
         <v>3</v>
@@ -1292,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="Q8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R8">
         <v>5</v>
@@ -1363,7 +1363,7 @@
         <v>5</v>
       </c>
       <c r="Q9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R9">
         <v>5</v>

</xml_diff>

<commit_message>
Fix : Wand_1_Epic_Skill이 SoundManager의 적용을 받지 않던 문제 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/WeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/WeaponDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28786B86-A66C-4E15-ACB1-2AB8F647A7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FB2797-D1A0-4617-8060-F5549304EFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="1005" windowWidth="37440" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
@@ -349,11 +349,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;color="red"&gt;스킬&lt;/color&gt; : 분노를 발산하여 일정 시간 동안 연사력이 올라갑니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GPT야, 활에 대한 이름을 지어줘.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color="red"&gt;스킬&lt;/color&gt; : 2초마다 주변을 향해 화살을 발사합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -724,7 +724,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1395,7 +1395,7 @@
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -1599,7 +1599,7 @@
         <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
         <v>55</v>

</xml_diff>